<commit_message>
Attendance up to date : Oct 11, 2021
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week8.xlsx
+++ b/Admin/Gaby/TimeSheet_Week8.xlsx
@@ -362,10 +362,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -512,7 +512,9 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
       <c r="E9" s="11"/>
@@ -521,7 +523,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13" t="n">
         <f aca="false">SUM(B9:H9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="9"/>
     </row>
@@ -582,7 +584,7 @@
       </c>
       <c r="B13" s="13" t="n">
         <f aca="false">SUM(B6:B12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="13" t="n">
         <f aca="false">SUM(C6:C12)</f>
@@ -610,7 +612,7 @@
       </c>
       <c r="I13" s="13" t="n">
         <f aca="false">SUM(I6:I12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Attendance up to 10/13
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week8.xlsx
+++ b/Admin/Gaby/TimeSheet_Week8.xlsx
@@ -362,10 +362,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -461,7 +461,9 @@
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
@@ -470,7 +472,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="13" t="n">
         <f aca="false">SUM(B6:H6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="9"/>
     </row>
@@ -497,14 +499,16 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
       <c r="G8" s="12"/>
       <c r="H8" s="11"/>
       <c r="I8" s="13" t="n">
         <f aca="false">SUM(B8:H8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -584,7 +588,7 @@
       </c>
       <c r="B13" s="13" t="n">
         <f aca="false">SUM(B6:B12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="13" t="n">
         <f aca="false">SUM(C6:C12)</f>
@@ -592,7 +596,7 @@
       </c>
       <c r="D13" s="13" t="n">
         <f aca="false">SUM(D6:D12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="13" t="n">
         <f aca="false">SUM(E6:E12)</f>
@@ -612,7 +616,7 @@
       </c>
       <c r="I13" s="13" t="n">
         <f aca="false">SUM(I6:I12)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Week 9 time sheet updated
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week8.xlsx
+++ b/Admin/Gaby/TimeSheet_Week8.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Read/Study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research/Personal Work</t>
   </si>
   <si>
     <t xml:space="preserve">Team Meting</t>
@@ -362,12 +365,12 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.17"/>
@@ -499,16 +502,18 @@
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
-      <c r="D8" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="I8" s="13" t="n">
         <f aca="false">SUM(B8:H8)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -516,11 +521,11 @@
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="11" t="n">
-        <v>1</v>
-      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
       <c r="G9" s="12"/>
@@ -535,7 +540,9 @@
       <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11"/>
+      <c r="B10" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -544,7 +551,7 @@
       <c r="H10" s="11"/>
       <c r="I10" s="13" t="n">
         <f aca="false">SUM(B10:H10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="9"/>
     </row>
@@ -583,45 +590,59 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="13" t="n">
-        <f aca="false">SUM(B6:B12)</f>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13" t="n">
+        <f aca="false">SUM(B13:H13)</f>
+        <v>1</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="13" t="n">
+        <f aca="false">SUM(B6:B13)</f>
         <v>2</v>
       </c>
-      <c r="C13" s="13" t="n">
-        <f aca="false">SUM(C6:C12)</f>
+      <c r="C14" s="13" t="n">
+        <f aca="false">SUM(C6:C13)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="13" t="n">
-        <f aca="false">SUM(D6:D12)</f>
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="n">
-        <f aca="false">SUM(E6:E12)</f>
+      <c r="D14" s="13" t="n">
+        <f aca="false">SUM(D6:D13)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="13" t="n">
+        <f aca="false">SUM(E6:E13)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="13" t="n">
-        <f aca="false">SUM(F6:F12)</f>
+      <c r="F14" s="13" t="n">
+        <f aca="false">SUM(F6:F13)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="13" t="n">
-        <f aca="false">SUM(G6:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="13" t="n">
-        <f aca="false">SUM(H6:H12)</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="13" t="n">
-        <f aca="false">SUM(I6:I12)</f>
+      <c r="G14" s="13" t="n">
+        <f aca="false">SUM(G6:G13)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>15</v>
+      <c r="H14" s="13" t="n">
+        <f aca="false">SUM(H6:H13)</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="13" t="n">
+        <f aca="false">SUM(I6:I13)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +675,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>